<commit_message>
aggiunto import per scuola intera fixate cose sull'import
</commit_message>
<xml_diff>
--- a/public/templates/template_studenti.xlsx
+++ b/public/templates/template_studenti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\web\mobilityamoci\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711C1B8A-F0F7-49A3-93B0-584732AADEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF1BD99-B424-4721-86BD-8165FDE2A6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-15250" windowWidth="38620" windowHeight="21100" xr2:uid="{4B8ABE6F-4219-49B4-8ECC-3D72D7A28498}"/>
   </bookViews>
@@ -716,7 +716,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -724,13 +724,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -742,14 +754,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Valore valido" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1064,7 +1079,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,43 +1100,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>220</v>
       </c>
     </row>

</xml_diff>